<commit_message>
update the package based on the 2nd revision
</commit_message>
<xml_diff>
--- a/Manuscript/Visualization/Fig1/Source_data_Figure1.xlsx
+++ b/Manuscript/Visualization/Fig1/Source_data_Figure1.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/be17a8240fc13af6/桌面/benchmarking/Github/upload_to_github/Visualization/Fig1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/be17a8240fc13af6/桌面/benchmarking/Nature_method/form_coauthors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_AD4DA82427541F7ACA7EB8FC280F3BFC6AE8DE12" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{166D2E55-948A-4B87-BB7C-A9B0AADCF3E2}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="11_AD4DA82427541F7ACA7EB8FC280F3BFC6AE8DE12" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9D1C5D4C-1150-4CCB-944D-1650EFFA10FB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Fig.1a" sheetId="2" r:id="rId1"/>
+    <sheet name="Fig.1b" sheetId="3" r:id="rId2"/>
+    <sheet name="Fig.1c" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Assembly_accession</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -122,16 +124,20 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>#The table was organized according to the profiling results in "Raw data and profiling results"</t>
+    <t>PathSeq-(default)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PathSeq-(corrected)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>#Comparison of profiling results of the simple simulated microbial community</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>PathSeq-(default)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PathSeq-(corrected)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t># This is a conceptual picture</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -243,34 +249,34 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -553,11 +559,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F77E53-B453-48AA-B31D-5B4A9872C25A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93D4848-BEA3-46DF-BDEB-EA23F91010DD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -581,247 +630,247 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="3"/>
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="9"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="6">
-        <v>398511</v>
-      </c>
-      <c r="C3" s="6">
-        <v>79885</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="8">
-        <v>4249248</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="9">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="H3" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="9">
-        <v>0.49859999999999999</v>
-      </c>
-      <c r="J3" s="10">
-        <v>0.49640000000000001</v>
-      </c>
-      <c r="K3" s="10">
-        <v>0.40959070972310502</v>
-      </c>
-      <c r="L3" s="10">
-        <v>0.27414742157431998</v>
-      </c>
-      <c r="M3" s="9">
-        <v>0.22787552174142758</v>
-      </c>
-      <c r="N3" s="9">
-        <v>7.0428488402810796E-2</v>
-      </c>
-      <c r="O3" s="9">
-        <v>0.33813019999999999</v>
-      </c>
-      <c r="P3" s="9">
-        <v>0.33570637660000002</v>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="6">
-        <v>362948</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1624</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="8">
-        <v>2133977</v>
-      </c>
-      <c r="F4" s="6">
-        <v>2</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="H4" s="9">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3">
+        <v>398511</v>
+      </c>
+      <c r="C4" s="3">
+        <v>79885</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5">
+        <v>4249248</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="H4" s="6">
         <v>0.5</v>
       </c>
-      <c r="I4" s="9">
-        <v>0.501</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0.49419999999999997</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0.48468382555912398</v>
-      </c>
-      <c r="L4" s="10">
-        <v>0.64597385315358202</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0.19860516722142971</v>
-      </c>
-      <c r="N4" s="9">
-        <v>8.0185273242810093E-2</v>
-      </c>
-      <c r="O4" s="9">
-        <v>0.66186980000000006</v>
-      </c>
-      <c r="P4" s="9">
-        <v>0.66429362339999998</v>
+      <c r="I4" s="6">
+        <v>0.49859999999999999</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.49640000000000001</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0.40959070972310502</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0.27414742157431998</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0.22787552174142758</v>
+      </c>
+      <c r="N4" s="6">
+        <v>7.0428488402810796E-2</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0.33813019999999999</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0.33570637660000002</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3">
+        <v>362948</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1624</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2133977</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="11">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="J5" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="K5" s="10">
-        <v>0.105</v>
-      </c>
-      <c r="L5" s="10">
-        <v>7.9878725272097939E-2</v>
-      </c>
-      <c r="M5" s="10">
-        <v>0.57299999999999995</v>
-      </c>
-      <c r="N5" s="10">
-        <v>0.85</v>
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.501</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.49419999999999997</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0.48468382555912398</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0.64597385315358202</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.19860516722142971</v>
+      </c>
+      <c r="N5" s="6">
+        <v>8.0185273242810093E-2</v>
       </c>
       <c r="O5" s="6">
-        <v>0</v>
+        <v>0.66186980000000006</v>
       </c>
       <c r="P5" s="6">
-        <v>0</v>
+        <v>0.66429362339999998</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0.105</v>
+      </c>
+      <c r="L6" s="7">
+        <v>7.9878725272097939E-2</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="N6" s="7">
+        <v>0.85</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>